<commit_message>
Refactor outlier detection configuration and handling
- Changed `file_path` to `dists_path` in `OutlierConfig` for clarity.
- Updated `OutlierDetector` to use `dists_path` for loading distance data.
- Modified `exclude_outliers` function signature to accept `dists_path`.
- Adjusted `BatchOrchestrator` to pass `out_base` and `tag` to `exclude_outliers`.
- Enhanced `OutlierHandler` to construct `dists_path` based on `out_base` and `tag`.
- Updated `StatisticsRunner` to include `mov` cloud data in statistics computation.
- Minor adjustments to logging for better traceability of point cloud processing.
</commit_message>
<xml_diff>
--- a/outputs/MARS_output/MARS_m3c2_stats_clouds.xlsx
+++ b/outputs/MARS_output/MARS_m3c2_stats_clouds.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sieglinde.hoedl\AI_Mars3D\src_uptodate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sieglinde.hoedl\AI_Mars3D\src_uptodate\outputs\MARS_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000"/>
   </bookViews>
   <sheets>
     <sheet name="CloudStats" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Timestamp</t>
   </si>
@@ -63,34 +63,34 @@
     <t>Z Q95</t>
   </si>
   <si>
-    <t>Mean NN Dist (1..6)</t>
-  </si>
-  <si>
-    <t>Mean Dist to 6-NN</t>
-  </si>
-  <si>
-    <t>Local Density Mean [pt/m^3]</t>
-  </si>
-  <si>
-    <t>Local Density Median [pt/m^3]</t>
-  </si>
-  <si>
-    <t>Local Density Q05 [pt/m^3]</t>
-  </si>
-  <si>
-    <t>Local Density Q95 [pt/m^3]</t>
-  </si>
-  <si>
-    <t>Roughness Mean [m]</t>
-  </si>
-  <si>
-    <t>Roughness Median [m]</t>
-  </si>
-  <si>
-    <t>Roughness Q05 [m]</t>
-  </si>
-  <si>
-    <t>Roughness Q95 [m]</t>
+    <t>Mean NN Dist All</t>
+  </si>
+  <si>
+    <t>Mean NN Dist k-th</t>
+  </si>
+  <si>
+    <t>Local Density Mean</t>
+  </si>
+  <si>
+    <t>Local Density Median</t>
+  </si>
+  <si>
+    <t>Local Density Q05</t>
+  </si>
+  <si>
+    <t>Local Density Q95</t>
+  </si>
+  <si>
+    <t>Roughness Mean</t>
+  </si>
+  <si>
+    <t>Roughness Median</t>
+  </si>
+  <si>
+    <t>Roughness Q05</t>
+  </si>
+  <si>
+    <t>Roughness Q95</t>
   </si>
   <si>
     <t>Linearity Mean</t>
@@ -109,6 +109,42 @@
   </si>
   <si>
     <t>Sphericity Median</t>
+  </si>
+  <si>
+    <t>Anisotropy Mean</t>
+  </si>
+  <si>
+    <t>Anisotropy Median</t>
+  </si>
+  <si>
+    <t>Omnivariance Mean</t>
+  </si>
+  <si>
+    <t>Omnivariance Median</t>
+  </si>
+  <si>
+    <t>Eigenentropy Mean</t>
+  </si>
+  <si>
+    <t>Eigenentropy Median</t>
+  </si>
+  <si>
+    <t>Curvature Mean</t>
+  </si>
+  <si>
+    <t>Curvature Median</t>
+  </si>
+  <si>
+    <t>Verticality Mean [deg]</t>
+  </si>
+  <si>
+    <t>Verticality Median [deg]</t>
+  </si>
+  <si>
+    <t>Verticality Q05 [deg]</t>
+  </si>
+  <si>
+    <t>Verticality Q95 [deg]</t>
   </si>
   <si>
     <t>Normal Std Angle [deg]</t>
@@ -489,19 +525,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ1"/>
+  <dimension ref="A1:AV1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -609,6 +644,42 @@
       </c>
       <c r="AJ1" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>